<commit_message>
actions: developing the initial content
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -1,22 +1,282 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Actions" sheetId="1" r:id="rId1"/>
+    <sheet name="Events" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Maintain unit tests</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Write unit tests</t>
+  </si>
+  <si>
+    <t>Continuous integration</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Description here</t>
+  </si>
+  <si>
+    <t>Rollover</t>
+  </si>
+  <si>
+    <t>Continuous integration II</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Next month: +1 Time</t>
+  </si>
+  <si>
+    <t>Next month: +3 Time</t>
+  </si>
+  <si>
+    <t>Next month: +2 Time</t>
+  </si>
+  <si>
+    <t>Next month: +4 Time</t>
+  </si>
+  <si>
+    <t>Card 22</t>
+  </si>
+  <si>
+    <t>Card 23</t>
+  </si>
+  <si>
+    <t>Card 29</t>
+  </si>
+  <si>
+    <t>Card 30</t>
+  </si>
+  <si>
+    <t>Card 31</t>
+  </si>
+  <si>
+    <t>Develop base features</t>
+  </si>
+  <si>
+    <t>Develop exciting features</t>
+  </si>
+  <si>
+    <t>Polishing features</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Risk assessment</t>
+  </si>
+  <si>
+    <t>Threat model</t>
+  </si>
+  <si>
+    <t>Incident response process</t>
+  </si>
+  <si>
+    <t>BEFORE EXCITING FEATURES: Your planning convinces the higher-ups of the risks, so they give you more resources. +1 Time</t>
+  </si>
+  <si>
+    <t>A threat model is a detailed planning technique used to examine how data flows in your system and how it is vulnerable to Spoofing, Tampering, Repudiation, Information Disclosure, Denial of Service, and Elevation of Privilege.</t>
+  </si>
+  <si>
+    <t>BEFORE EXCITING FEATURES: You catch a lot of bugs in the base feature set. +2 Time</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Injection</t>
+  </si>
+  <si>
+    <t>Learn memory corruption</t>
+  </si>
+  <si>
+    <t>Your team trains on memory corruption vulnerabilities that plague native languages (C/C++), such as buffer overflows and format string vulnerabilities.</t>
+  </si>
+  <si>
+    <t>Enable ASLR</t>
+  </si>
+  <si>
+    <t>Your team employs Address Space Layout Randomization. This makes memory corruption vulnerabilities difficult to exploit, but not impossible for a determined attacker.</t>
+  </si>
+  <si>
+    <t>Crash reporting system</t>
+  </si>
+  <si>
+    <t>You make a feature that records when the product crashes and reports it back to the dev team. These crashes are often the first sign of a devastating memory corruption vulnerability.</t>
+  </si>
+  <si>
+    <t>BEFORE BASE FEATURES: You caught some lazy coders early. +2 Time</t>
+  </si>
+  <si>
+    <t>Minimum viable product</t>
+  </si>
+  <si>
+    <t>You build a prototype to prove its capability to investors. 
+This is part of your routine development and you will have to do this at some point.</t>
+  </si>
+  <si>
+    <t>You build out the main features of the system.
+This is part of your routine development and you will have to do this at some point.</t>
+  </si>
+  <si>
+    <t>You develop features that separate your product from the competition.
+This is part of your routine development and you will have to do this at some point.</t>
+  </si>
+  <si>
+    <t>You prepare your product for widespread launch.
+This is part of your routine development and you will have to do this at some point.</t>
+  </si>
+  <si>
+    <t>Fuzz testing</t>
+  </si>
+  <si>
+    <t>You employ a massive artificial intelligence system to develop potential exploits and find memory corruption vulnerabilities.</t>
+  </si>
+  <si>
+    <t>Learn basic injection</t>
+  </si>
+  <si>
+    <t>Your team trains on injection vulnerabilities found in many technologies, such as SQL-injection, Cross-site scripting, and OS command injection.</t>
+  </si>
+  <si>
+    <t>Distrustful decomposition</t>
+  </si>
+  <si>
+    <t>More injection</t>
+  </si>
+  <si>
+    <t>Not sure about this yet</t>
+  </si>
+  <si>
+    <t>Input validation</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Password improvements</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>You secure the way your product handles passwords, such as hashing with salt.</t>
+  </si>
+  <si>
+    <t>Two-factor authentication</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>You develop access control features that limit what authenticated users can do.</t>
+  </si>
+  <si>
+    <t>Audit Logs</t>
+  </si>
+  <si>
+    <t>Deploy SSL</t>
+  </si>
+  <si>
+    <t>Enable Secure Sockets Layer to any networked traffic on your application.</t>
+  </si>
+  <si>
+    <t>BEFORE EXCITING FEATURES: You catch a lot of bugs in the base feature set. +1 Time</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Now that you have a good idea of the threats that face your product, you can react to exploits in an orderly manner.</t>
+  </si>
+  <si>
+    <t>Abuse and misuse cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You explore your risks more by writing and ranking potential compromise scenarios. </t>
+  </si>
+  <si>
+    <t>You document and discuss as a team the important assets your product is protecting, and how easy those assets might be to compromise.</t>
+  </si>
+  <si>
+    <t>Your team is now in the habit of writing tests, so these are much easier to write.</t>
+  </si>
+  <si>
+    <t>Your team write an automated test suite, which allow developers to check their own work. This builds up a defensive mindset, and makes big code changes easier to make later on.
+Cost is 5 if Base features are already developed, 6 for Exciting Features.</t>
+  </si>
+  <si>
+    <t>You set up a build server that automatically runs your unit tests after every change, notifying developers of potential problems early.</t>
+  </si>
+  <si>
+    <t>Your build server requires little maintenance at this point.</t>
+  </si>
+  <si>
+    <t>You add a subsystem for defensively checking that user input is not malformed. 
+Cost is 2 if Base features are already developed</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,14 +304,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +419,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,12 +627,628 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>